<commit_message>
New text and start of the treemap.
</commit_message>
<xml_diff>
--- a/data/Number for migrant interactive.xlsx
+++ b/data/Number for migrant interactive.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="5080" windowWidth="25240" windowHeight="21180" activeTab="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="216">
   <si>
     <t>Belgium</t>
   </si>
@@ -663,6 +663,15 @@
   </si>
   <si>
     <t>Namibia</t>
+  </si>
+  <si>
+    <t>KOS</t>
+  </si>
+  <si>
+    <t>ESH</t>
+  </si>
+  <si>
+    <t>UNK</t>
   </si>
 </sst>
 </file>
@@ -7740,7 +7749,7 @@
   <dimension ref="A1:L158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D157"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7806,9 +7815,8 @@
       <c r="B3">
         <v>96800</v>
       </c>
-      <c r="C3" t="str">
-        <f>VLOOKUP(A3,[1]Eurostat_lookup!$B$2:$F$234,5,0)</f>
-        <v>UNK</v>
+      <c r="C3" t="s">
+        <v>213</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D66" si="0">VLOOKUP(A3,$I$2:$L$158,4,0)</f>
@@ -8198,9 +8206,8 @@
       <c r="B17">
         <v>13905</v>
       </c>
-      <c r="C17" t="str">
-        <f>VLOOKUP(A17,[1]Eurostat_lookup!$B$2:$F$234,5,0)</f>
-        <v>N</v>
+      <c r="C17" t="s">
+        <v>215</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -9283,20 +9290,6 @@
       </c>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" t="s">
-        <v>41</v>
-      </c>
-      <c r="B56">
-        <v>890</v>
-      </c>
-      <c r="C56" t="str">
-        <f>VLOOKUP(A56,[1]Eurostat_lookup!$B$2:$F$234,5,0)</f>
-        <v>EU28</v>
-      </c>
-      <c r="D56">
-        <f t="shared" si="0"/>
-        <v>1.5748031496062991</v>
-      </c>
       <c r="I56" t="s">
         <v>120</v>
       </c>
@@ -9625,9 +9618,8 @@
       <c r="B68">
         <v>590</v>
       </c>
-      <c r="C68" t="str">
-        <f>VLOOKUP(A68,[1]Eurostat_lookup!$B$2:$F$234,5,0)</f>
-        <v>WSA</v>
+      <c r="C68" t="s">
+        <v>214</v>
       </c>
       <c r="D68">
         <f t="shared" si="1"/>

</xml_diff>